<commit_message>
Update gold data automatically
</commit_message>
<xml_diff>
--- a/data/gold_data.xlsx
+++ b/data/gold_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1464"/>
+  <dimension ref="A1:I1465"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39985,6 +39985,33 @@
       </c>
       <c r="I1464" t="inlineStr"/>
     </row>
+    <row r="1465">
+      <c r="A1465" s="2" t="n">
+        <v>45954</v>
+      </c>
+      <c r="B1465" t="n">
+        <v>4144</v>
+      </c>
+      <c r="C1465" t="n">
+        <v>4159</v>
+      </c>
+      <c r="D1465" t="n">
+        <v>4055.699951171875</v>
+      </c>
+      <c r="E1465" t="n">
+        <v>4142.2998046875</v>
+      </c>
+      <c r="F1465" t="n">
+        <v>215904</v>
+      </c>
+      <c r="G1465" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1465" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1465" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>